<commit_message>
Rio2016 match Womens Asia Finals added data
</commit_message>
<xml_diff>
--- a/Metadata_youtube.xlsx
+++ b/Metadata_youtube.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vatsa\TT\SpinClassifier\TT_spin_classifier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vyas Raina\Documents\Software_Projects\TT\Model\TT_spin_classifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7507D210-1006-4F09-B67A-E44B1DD8D9C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B3AF2E-BE88-4D3B-B140-53D767391E37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A9C22603-7041-48CF-BF61-745C2CAF1C55}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A9C22603-7041-48CF-BF61-745C2CAF1C55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="175">
   <si>
     <t>ID</t>
   </si>
@@ -414,18 +408,9 @@
     <t>1:08.74</t>
   </si>
   <si>
-    <t xml:space="preserve">2019 Qatar Open </t>
-  </si>
-  <si>
     <t>clip42</t>
   </si>
   <si>
-    <t xml:space="preserve">2020 Qatar Open </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021 Qatar Open </t>
-  </si>
-  <si>
     <t>clip43</t>
   </si>
   <si>
@@ -438,21 +423,6 @@
     <t>1:27.42</t>
   </si>
   <si>
-    <t xml:space="preserve">2022 Qatar Open </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023 Qatar Open </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024 Qatar Open </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025 Qatar Open </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2026 Qatar Open </t>
-  </si>
-  <si>
     <t>clip45</t>
   </si>
   <si>
@@ -486,28 +456,100 @@
     <t>16:54.47</t>
   </si>
   <si>
-    <t xml:space="preserve">2027 Qatar Open </t>
-  </si>
-  <si>
     <t>clip50</t>
   </si>
   <si>
     <t>clip51</t>
   </si>
   <si>
-    <t xml:space="preserve">2028 Qatar Open </t>
-  </si>
-  <si>
     <t>18:02.80</t>
   </si>
   <si>
     <t>clip52</t>
   </si>
   <si>
-    <t xml:space="preserve">2029 Qatar Open </t>
-  </si>
-  <si>
     <t>22:58.20</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9_x90IzBMCA</t>
+  </si>
+  <si>
+    <t>Rio2016 Asia Qualifiers</t>
+  </si>
+  <si>
+    <t>Kim Olga</t>
+  </si>
+  <si>
+    <t>Neda Shahsavari</t>
+  </si>
+  <si>
+    <t>clip53</t>
+  </si>
+  <si>
+    <t>0:39.20</t>
+  </si>
+  <si>
+    <t>clip54</t>
+  </si>
+  <si>
+    <t>clip55</t>
+  </si>
+  <si>
+    <t>clip56</t>
+  </si>
+  <si>
+    <t>clip57</t>
+  </si>
+  <si>
+    <t>clip58</t>
+  </si>
+  <si>
+    <t>clip59</t>
+  </si>
+  <si>
+    <t>clip60</t>
+  </si>
+  <si>
+    <t>0:43.46</t>
+  </si>
+  <si>
+    <t>1:15.53</t>
+  </si>
+  <si>
+    <t>CHOP</t>
+  </si>
+  <si>
+    <t>1:16.63</t>
+  </si>
+  <si>
+    <t>3:56.96</t>
+  </si>
+  <si>
+    <t>4:21.36</t>
+  </si>
+  <si>
+    <t>clip61</t>
+  </si>
+  <si>
+    <t>clip62</t>
+  </si>
+  <si>
+    <t>clip63</t>
+  </si>
+  <si>
+    <t>6:41.23</t>
+  </si>
+  <si>
+    <t>7:49.50</t>
+  </si>
+  <si>
+    <t>18:53.33</t>
+  </si>
+  <si>
+    <t>23:59.20</t>
+  </si>
+  <si>
+    <t>53:47.10</t>
   </si>
 </sst>
 </file>
@@ -585,8 +627,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{66369352-10E0-472D-8237-914C7EC25ECA}" name="Table1" displayName="Table1" ref="A1:K61" totalsRowShown="0">
-  <autoFilter ref="A1:K61" xr:uid="{81BED2F6-A735-48E8-8312-3441EAEEF1B9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{66369352-10E0-472D-8237-914C7EC25ECA}" name="Table1" displayName="Table1" ref="A1:K327" totalsRowShown="0">
+  <autoFilter ref="A1:K327" xr:uid="{81BED2F6-A735-48E8-8312-3441EAEEF1B9}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{DF59981D-0EFF-443B-97EC-88206A26AB07}" name="ID"/>
     <tableColumn id="2" xr3:uid="{85D201EA-997B-46FC-ABB5-FBAEB62C900B}" name="FH/BH"/>
@@ -901,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172545AB-FD49-4BA5-8D0D-D9C0E3079292}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2393,7 +2435,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B43" t="s">
         <v>21</v>
@@ -2402,7 +2444,7 @@
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E43" t="s">
         <v>123</v>
@@ -2428,7 +2470,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
@@ -2437,7 +2479,7 @@
         <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E44" t="s">
         <v>123</v>
@@ -2458,12 +2500,12 @@
         <v>121</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
         <v>21</v>
@@ -2472,7 +2514,7 @@
         <v>26</v>
       </c>
       <c r="D45" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E45" t="s">
         <v>123</v>
@@ -2493,12 +2535,12 @@
         <v>121</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
         <v>21</v>
@@ -2507,7 +2549,7 @@
         <v>49</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E46" t="s">
         <v>123</v>
@@ -2528,12 +2570,12 @@
         <v>121</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B47" t="s">
         <v>21</v>
@@ -2542,7 +2584,7 @@
         <v>30</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E47" t="s">
         <v>123</v>
@@ -2563,12 +2605,12 @@
         <v>121</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s">
         <v>20</v>
@@ -2577,7 +2619,7 @@
         <v>36</v>
       </c>
       <c r="D48" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="E48" t="s">
         <v>123</v>
@@ -2598,12 +2640,12 @@
         <v>121</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B49" t="s">
         <v>20</v>
@@ -2612,7 +2654,7 @@
         <v>32</v>
       </c>
       <c r="D49" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="E49" t="s">
         <v>123</v>
@@ -2633,12 +2675,12 @@
         <v>121</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B50" t="s">
         <v>20</v>
@@ -2647,7 +2689,7 @@
         <v>57</v>
       </c>
       <c r="D50" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="E50" t="s">
         <v>123</v>
@@ -2668,12 +2710,12 @@
         <v>121</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B51" t="s">
         <v>20</v>
@@ -2682,7 +2724,7 @@
         <v>41</v>
       </c>
       <c r="D51" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="E51" t="s">
         <v>123</v>
@@ -2703,12 +2745,12 @@
         <v>121</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B52" t="s">
         <v>21</v>
@@ -2717,7 +2759,7 @@
         <v>36</v>
       </c>
       <c r="D52" t="s">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="E52" t="s">
         <v>123</v>
@@ -2738,12 +2780,12 @@
         <v>121</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
         <v>21</v>
@@ -2752,7 +2794,7 @@
         <v>41</v>
       </c>
       <c r="D53" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="E53" t="s">
         <v>124</v>
@@ -2773,12 +2815,400 @@
         <v>121</v>
       </c>
       <c r="K53" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>152</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" t="s">
+        <v>149</v>
+      </c>
+      <c r="E54" t="s">
+        <v>150</v>
+      </c>
+      <c r="F54" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" t="s">
+        <v>66</v>
+      </c>
+      <c r="H54" t="s">
+        <v>151</v>
+      </c>
+      <c r="I54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" t="s">
+        <v>150</v>
+      </c>
+      <c r="F55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" t="s">
+        <v>66</v>
+      </c>
+      <c r="H55" t="s">
+        <v>151</v>
+      </c>
+      <c r="I55" t="s">
+        <v>13</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>155</v>
+      </c>
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" t="s">
+        <v>149</v>
+      </c>
+      <c r="E56" t="s">
+        <v>150</v>
+      </c>
+      <c r="F56" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" t="s">
+        <v>66</v>
+      </c>
+      <c r="H56" t="s">
+        <v>151</v>
+      </c>
+      <c r="I56" t="s">
+        <v>13</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>156</v>
+      </c>
+      <c r="B57" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" t="s">
+        <v>163</v>
+      </c>
+      <c r="D57" t="s">
+        <v>149</v>
+      </c>
+      <c r="E57" t="s">
+        <v>150</v>
+      </c>
+      <c r="F57" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" t="s">
+        <v>66</v>
+      </c>
+      <c r="H57" t="s">
+        <v>151</v>
+      </c>
+      <c r="I57" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>157</v>
+      </c>
+      <c r="B58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" t="s">
+        <v>163</v>
+      </c>
+      <c r="D58" t="s">
+        <v>149</v>
+      </c>
+      <c r="E58" t="s">
+        <v>150</v>
+      </c>
+      <c r="F58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" t="s">
+        <v>66</v>
+      </c>
+      <c r="H58" t="s">
+        <v>151</v>
+      </c>
+      <c r="I58" t="s">
+        <v>13</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>158</v>
+      </c>
+      <c r="B59" t="s">
+        <v>21</v>
+      </c>
+      <c r="C59" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59" t="s">
+        <v>149</v>
+      </c>
+      <c r="E59" t="s">
+        <v>150</v>
+      </c>
+      <c r="F59" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" t="s">
+        <v>66</v>
+      </c>
+      <c r="H59" t="s">
+        <v>151</v>
+      </c>
+      <c r="I59" t="s">
+        <v>13</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>159</v>
+      </c>
+      <c r="B60" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" t="s">
+        <v>46</v>
+      </c>
+      <c r="D60" t="s">
+        <v>149</v>
+      </c>
+      <c r="E60" t="s">
+        <v>151</v>
+      </c>
+      <c r="F60" t="s">
+        <v>37</v>
+      </c>
+      <c r="G60" t="s">
+        <v>66</v>
+      </c>
+      <c r="H60" t="s">
+        <v>150</v>
+      </c>
+      <c r="I60" t="s">
+        <v>13</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>160</v>
+      </c>
+      <c r="B61" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61" t="s">
+        <v>149</v>
+      </c>
+      <c r="E61" t="s">
+        <v>151</v>
+      </c>
+      <c r="F61" t="s">
+        <v>37</v>
+      </c>
+      <c r="G61" t="s">
+        <v>66</v>
+      </c>
+      <c r="H61" t="s">
+        <v>150</v>
+      </c>
+      <c r="I61" t="s">
+        <v>13</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>167</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62" t="s">
+        <v>36</v>
+      </c>
+      <c r="D62" t="s">
+        <v>149</v>
+      </c>
+      <c r="E62" t="s">
+        <v>151</v>
+      </c>
+      <c r="F62" t="s">
+        <v>37</v>
+      </c>
+      <c r="G62" t="s">
+        <v>66</v>
+      </c>
+      <c r="H62" t="s">
+        <v>150</v>
+      </c>
+      <c r="I62" t="s">
+        <v>13</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>168</v>
+      </c>
+      <c r="B63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" t="s">
+        <v>149</v>
+      </c>
+      <c r="E63" t="s">
+        <v>151</v>
+      </c>
+      <c r="F63" t="s">
+        <v>37</v>
+      </c>
+      <c r="G63" t="s">
+        <v>66</v>
+      </c>
+      <c r="H63" t="s">
+        <v>150</v>
+      </c>
+      <c r="I63" t="s">
+        <v>13</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>169</v>
+      </c>
+      <c r="B64" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" t="s">
+        <v>57</v>
+      </c>
+      <c r="D64" t="s">
+        <v>149</v>
+      </c>
+      <c r="E64" t="s">
+        <v>151</v>
+      </c>
+      <c r="F64" t="s">
+        <v>37</v>
+      </c>
+      <c r="G64" t="s">
+        <v>66</v>
+      </c>
+      <c r="H64" t="s">
+        <v>150</v>
+      </c>
+      <c r="I64" t="s">
+        <v>13</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I327 H328:H1048576" xr:uid="{A1296B59-2288-4745-AA5B-44A4FA2D861F}">
+      <formula1>"LEFT,RIGHT,CENTRE"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{2E77D5AE-80A7-4DAD-A997-2F60E5ED1395}">
       <formula1>"FH,BH"</formula1>
     </dataValidation>
@@ -2787,9 +3217,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{F76C36A9-DCB9-4CC9-8BAC-E39A10C32D78}">
       <formula1>"SPEED DRIVE,LOOP DRIVE,FLICK,SMASH,SLICE,CHOP,BLOCK,PUSH-BLOCK,SIDE DRIVE,LOB,STOP"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H62:H1048576 I1:I61" xr:uid="{A1296B59-2288-4745-AA5B-44A4FA2D861F}">
-      <formula1>"LEFT,RIGHT,CENTRE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{101F5CD2-4675-487D-B173-6B9245FF1FAF}">
       <formula1>"YES,NO"</formula1>
@@ -2825,11 +3252,16 @@
     <hyperlink ref="J51" r:id="rId27" xr:uid="{163F6B2E-E6AF-4E59-B7E7-607BE17BD9A8}"/>
     <hyperlink ref="J52" r:id="rId28" xr:uid="{4DD23F56-3436-4392-BA89-DC2094AF04B4}"/>
     <hyperlink ref="J53" r:id="rId29" xr:uid="{36C1A1AC-9E66-4565-A4A0-317074969782}"/>
+    <hyperlink ref="J54" r:id="rId30" xr:uid="{A306EBEC-874D-473D-B16B-BB3C6AEF89DC}"/>
+    <hyperlink ref="J55:J59" r:id="rId31" display="https://www.youtube.com/watch?v=9_x90IzBMCA" xr:uid="{46E66AA7-C776-4458-B2CF-CE69278E887D}"/>
+    <hyperlink ref="J60:J62" r:id="rId32" display="https://www.youtube.com/watch?v=9_x90IzBMCA" xr:uid="{D068006E-93C9-4A9A-9CE8-A8F18FE7340F}"/>
+    <hyperlink ref="J63" r:id="rId33" xr:uid="{F44587FB-19D6-4FB1-AD59-54847C69E2F6}"/>
+    <hyperlink ref="J64" r:id="rId34" xr:uid="{552C07A4-CD4B-49CF-B27A-7D428157C1B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId30"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId35"/>
   <tableParts count="1">
-    <tablePart r:id="rId31"/>
+    <tablePart r:id="rId36"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>